<commit_message>
I am still weeding through and spending way tooooo much time looking into covariance. I should probably just quit and move on but I havent yet
</commit_message>
<xml_diff>
--- a/Data/2023_09_08_final_long_format_adsorption_titers.xlsx
+++ b/Data/2023_09_08_final_long_format_adsorption_titers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicrobeJ\Documents\R_projects\with_trainees\PhiCB5-AbsorptionAssay\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA7B570-ABE0-4F8F-8FFC-0147FA2D5DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B7753-BF78-4B81-B573-ACC5C401653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15870" yWindow="225" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27420" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final_long_format_titer_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="9">
   <si>
     <t>Sample</t>
   </si>
@@ -888,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +944,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>44965</v>
@@ -953,26 +953,26 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>92</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>191</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>44970</v>
@@ -981,12 +981,12 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>44970</v>
@@ -995,12 +995,12 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>44970</v>
@@ -1009,12 +1009,12 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>198</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>44970</v>
@@ -1023,12 +1023,12 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>310</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>44970</v>
@@ -1037,12 +1037,12 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>291</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
         <v>44970</v>
@@ -1051,12 +1051,12 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>160</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>44970</v>
@@ -1065,12 +1065,12 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>298</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1">
         <v>44970</v>
@@ -1079,12 +1079,12 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>125</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
         <v>44970</v>
@@ -1093,12 +1093,12 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>44970</v>
@@ -1107,12 +1107,12 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>44970</v>
@@ -1121,26 +1121,26 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>145</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>44965</v>
+        <v>44970</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
         <v>44965</v>
@@ -1149,12 +1149,12 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>44965</v>
@@ -1163,40 +1163,40 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>172</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21">
-        <v>198</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22" s="1">
         <v>44970</v>
@@ -1205,12 +1205,12 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>126</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1">
         <v>44970</v>
@@ -1219,12 +1219,12 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1">
         <v>44970</v>
@@ -1233,12 +1233,12 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>299</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1">
         <v>44970</v>
@@ -1247,12 +1247,12 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>318</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="1">
         <v>44970</v>
@@ -1261,12 +1261,12 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>181</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1">
         <v>44970</v>
@@ -1275,12 +1275,12 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>298</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1">
         <v>44970</v>
@@ -1289,12 +1289,12 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>124</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1">
         <v>44970</v>
@@ -1303,12 +1303,12 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>130</v>
+        <v>298</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1">
         <v>44970</v>
@@ -1317,12 +1317,12 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>75</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1">
         <v>44970</v>
@@ -1331,40 +1331,40 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1">
-        <v>44965</v>
+        <v>44970</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>178</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1">
-        <v>44965</v>
+        <v>44970</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>187</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B34" s="1">
         <v>44965</v>
@@ -1373,54 +1373,54 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>76</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B35" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36">
-        <v>195</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1">
-        <v>44970</v>
+        <v>44965</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <v>125</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B38" s="1">
         <v>44970</v>
@@ -1429,12 +1429,12 @@
         <v>3</v>
       </c>
       <c r="D38">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" s="1">
         <v>44970</v>
@@ -1443,12 +1443,12 @@
         <v>3</v>
       </c>
       <c r="D39">
-        <v>296</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1">
         <v>44970</v>
@@ -1457,12 +1457,12 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <v>308</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1">
         <v>44970</v>
@@ -1471,12 +1471,12 @@
         <v>3</v>
       </c>
       <c r="D41">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1">
         <v>44970</v>
@@ -1485,12 +1485,12 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1">
         <v>44970</v>
@@ -1499,12 +1499,12 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <v>125</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1">
         <v>44970</v>
@@ -1513,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <v>131</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,49 +1527,49 @@
         <v>3</v>
       </c>
       <c r="D45">
-        <v>144</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1">
-        <v>45178</v>
+        <v>44970</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1">
-        <v>45178</v>
+        <v>44970</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47">
-        <v>85</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" s="1">
-        <v>45178</v>
+        <v>44970</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48">
-        <v>122</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,13 +1577,13 @@
         <v>8</v>
       </c>
       <c r="B49" s="1">
-        <v>45179</v>
+        <v>45178</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>162</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,13 +1591,13 @@
         <v>8</v>
       </c>
       <c r="B50" s="1">
-        <v>45179</v>
+        <v>45178</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
       <c r="D50">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,13 +1605,13 @@
         <v>8</v>
       </c>
       <c r="B51" s="1">
-        <v>45179</v>
+        <v>45178</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
       <c r="D51">
-        <v>81</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,13 +1619,13 @@
         <v>8</v>
       </c>
       <c r="B52" s="1">
-        <v>45181</v>
+        <v>45179</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,13 +1633,13 @@
         <v>8</v>
       </c>
       <c r="B53" s="1">
-        <v>45181</v>
+        <v>45179</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,13 +1647,223 @@
         <v>8</v>
       </c>
       <c r="B54" s="1">
+        <v>45179</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1">
         <v>45181</v>
       </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="D54">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45181</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1">
+        <v>45181</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
         <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1">
+        <v>45177</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="1">
+        <v>45177</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45177</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1">
+        <v>45178</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="1">
+        <v>45178</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1">
+        <v>45178</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="1">
+        <v>45179</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1">
+        <v>45179</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="1">
+        <v>45179</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45181</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45181</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="1">
+        <v>45181</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>